<commit_message>
fixed an issue caused by excel autoscaling
</commit_message>
<xml_diff>
--- a/KPI-visualization-tool.xlsx
+++ b/KPI-visualization-tool.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\campcapp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\campcapp\KPI-Visualization-Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71E0308C-1017-4D50-B30A-DA4F26E21688}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9D41B2-DAA8-432D-AE96-166DC7B92BEE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,18 +27,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>KPI Bands</t>
-  </si>
-  <si>
-    <t>Performance out of 100</t>
   </si>
   <si>
     <t>Speedometer</t>
   </si>
   <si>
     <t>Bar chart</t>
+  </si>
+  <si>
+    <t>Preformance out of 100</t>
+  </si>
+  <si>
+    <t>KPI Bands out of 100</t>
   </si>
 </sst>
 </file>
@@ -212,7 +215,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$2</c:f>
+              <c:f>Sheet1!$M$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -293,7 +296,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$6</c:f>
+              <c:f>Sheet1!$M$4:$M$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -337,12 +340,9 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$2</c:f>
+              <c:f>Sheet1!$N$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Performance out of 100</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -416,18 +416,18 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$3:$I$6</c:f>
+              <c:f>Sheet1!$N$4:$N$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>74</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>124</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -533,7 +533,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$3</c:f>
+              <c:f>Sheet1!$M$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -564,7 +564,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$4</c:f>
+              <c:f>Sheet1!$M$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -595,7 +595,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$5</c:f>
+              <c:f>Sheet1!$M$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -715,10 +715,20 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.6478567470727058E-2"/>
+          <c:y val="6.1148345799366892E-2"/>
+          <c:w val="0.82426954749461445"/>
+          <c:h val="0.8777033084012662"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="percentStacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -733,12 +743,12 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$3</c:f>
+              <c:f>Sheet1!$P$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -757,14 +767,16 @@
               <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$4</c:f>
+              <c:f>Sheet1!$P$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -784,9 +796,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
+            <a:noFill/>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -797,13 +807,6 @@
             <c:idx val="0"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-96FA-4CEE-B31E-B463E6BDC668}"/>
@@ -812,12 +815,12 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$5</c:f>
+              <c:f>Sheet1!$P$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>75</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -848,12 +851,26 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="577907600"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -863,10 +880,12 @@
         <c:axId val="577907600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -890,7 +909,7 @@
     <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -2046,25 +2065,25 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="303">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -2072,7 +2091,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2080,22 +2099,22 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2103,14 +2122,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="75000"/>
         <a:lumOff val="25000"/>
       </a:schemeClr>
@@ -2147,35 +2166,45 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2187,30 +2216,34 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="15875">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2226,16 +2259,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2243,14 +2275,14 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2261,9 +2293,9 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2275,12 +2307,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -2294,14 +2326,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2313,13 +2345,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
     </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
@@ -2327,12 +2366,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2346,12 +2385,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
@@ -2365,14 +2404,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2384,12 +2423,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -2403,39 +2442,68 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+    </cs:spPr>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:plotArea3D>
   <cs:seriesAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2443,12 +2511,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
@@ -2461,13 +2529,13 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2476,14 +2544,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2492,7 +2559,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -2504,7 +2571,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2512,9 +2579,9 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2526,11 +2593,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2538,13 +2616,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="ltDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
@@ -2629,13 +2714,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>13512</xdr:colOff>
+      <xdr:colOff>13513</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>4731</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>628245</xdr:colOff>
+      <xdr:colOff>635000</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>80932</xdr:rowOff>
     </xdr:to>
@@ -2965,44 +3050,40 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:K28"/>
+  <dimension ref="B2:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="8" width="9.1796875" customWidth="1"/>
+    <col min="2" max="7" width="9.1796875" customWidth="1"/>
+    <col min="8" max="8" width="21.1796875" customWidth="1"/>
     <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3"/>
       <c r="H2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
-        <v>1</v>
+      <c r="P2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -3011,72 +3092,92 @@
         <v>25</v>
       </c>
       <c r="I3">
-        <v>74</v>
+        <v>90</v>
       </c>
-      <c r="K3">
-        <v>23</v>
+      <c r="M3" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="6"/>
       <c r="H4">
-        <v>50</v>
+        <v>75</v>
       </c>
-      <c r="I4">
-        <v>2</v>
+      <c r="M4">
+        <f>H3</f>
+        <v>25</v>
       </c>
-      <c r="K4">
-        <v>2</v>
+      <c r="N4">
+        <f>I3</f>
+        <v>90</v>
+      </c>
+      <c r="P4">
+        <f>I3</f>
+        <v>90</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="6"/>
       <c r="H5">
-        <v>25</v>
+        <v>100</v>
       </c>
-      <c r="I5">
-        <f>200-I3-I4</f>
-        <v>124</v>
+      <c r="M5">
+        <f>H4-H3</f>
+        <v>50</v>
       </c>
-      <c r="K5">
-        <f>100-K3-K4</f>
-        <v>75</v>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
-      <c r="H6">
-        <v>100</v>
+      <c r="M6">
+        <f>H5-H4</f>
+        <v>25</v>
+      </c>
+      <c r="N6">
+        <f>200-N4-N5</f>
+        <v>108</v>
+      </c>
+      <c r="P6">
+        <f>100-P4-P5</f>
+        <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
+      <c r="M7">
+        <v>100</v>
+      </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>

</xml_diff>

<commit_message>
added instructions, fixed a mistake
</commit_message>
<xml_diff>
--- a/KPI-visualization-tool.xlsx
+++ b/KPI-visualization-tool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\campcapp\KPI-Visualization-Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9D41B2-DAA8-432D-AE96-166DC7B92BEE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5186490D-D682-4F47-8668-0B33E00E4345}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -79,101 +79,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,13 +334,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>90</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>108</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -508,10 +421,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.581033892502567E-3"/>
-          <c:y val="6.4814496441219956E-3"/>
-          <c:w val="0.99741896610749747"/>
-          <c:h val="0.99351855035587799"/>
+          <c:x val="0"/>
+          <c:y val="0"/>
+          <c:w val="1"/>
+          <c:h val="1"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -554,10 +467,16 @@
           <c:order val="1"/>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FFFF00"/>
+              <a:srgbClr val="FFFF00">
+                <a:alpha val="96000"/>
+              </a:srgbClr>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:alpha val="91000"/>
+                </a:schemeClr>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -748,7 +667,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>90</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -820,7 +739,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -851,20 +770,6 @@
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -908,12 +813,7 @@
   <c:spPr>
     <a:noFill/>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2676,15 +2576,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>148618</xdr:colOff>
+      <xdr:colOff>6881</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>27021</xdr:rowOff>
+      <xdr:rowOff>47952</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>588254</xdr:colOff>
+      <xdr:colOff>446987</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>9728</xdr:rowOff>
+      <xdr:rowOff>30659</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2713,16 +2613,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>13513</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>362420</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>4731</xdr:rowOff>
+      <xdr:rowOff>12570</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
+      <xdr:colOff>408216</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>80932</xdr:rowOff>
+      <xdr:rowOff>88771</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3050,9 +2950,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:P28"/>
+  <dimension ref="A2:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -3065,11 +2965,11 @@
     <col min="10" max="10" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
       <c r="H2" t="s">
         <v>4</v>
       </c>
@@ -3083,26 +2983,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
       <c r="H3">
         <v>25</v>
       </c>
       <c r="I3">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="M3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
       <c r="H4">
         <v>75</v>
       </c>
@@ -3112,18 +3012,18 @@
       </c>
       <c r="N4">
         <f>I3</f>
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="P4">
-        <f>I3</f>
-        <v>90</v>
+        <f>I3-2</f>
+        <v>73</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="H5">
         <v>100</v>
       </c>
@@ -3138,146 +3038,220 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
       <c r="M6">
         <f>H5-H4</f>
         <v>25</v>
       </c>
       <c r="N6">
         <f>200-N4-N5</f>
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="P6">
         <f>100-P4-P5</f>
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="M7">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="3"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="6"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="6"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="6"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B21" s="4"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="6"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B22" s="4"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="6"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="6"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="6"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B26" s="4"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="6"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B27" s="4"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="6"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="2"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="9"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="2"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>